<commit_message>
updated figures and stats
</commit_message>
<xml_diff>
--- a/Data/arcbt.xlsx
+++ b/Data/arcbt.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code Projects\Code Blue Training\R-Stats\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code Projects\Code Blue Training Edits\code-seminar-analysis\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8652F2D0-50B8-42B7-8234-89B4F889B910}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2DFE85B-990E-4D75-8E69-F1095B8AA890}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{8A6DFDBA-5F4B-4D43-9220-6C264F66262A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21600" xr2:uid="{8A6DFDBA-5F4B-4D43-9220-6C264F66262A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>pre_con_code</t>
   </si>
@@ -75,6 +75,84 @@
   </si>
   <si>
     <t>q_right</t>
+  </si>
+  <si>
+    <t>D6484</t>
+  </si>
+  <si>
+    <t>b6307</t>
+  </si>
+  <si>
+    <t>J8896</t>
+  </si>
+  <si>
+    <t>D9435</t>
+  </si>
+  <si>
+    <t>S8428</t>
+  </si>
+  <si>
+    <t>G0883</t>
+  </si>
+  <si>
+    <t>K7146</t>
+  </si>
+  <si>
+    <t>L9203</t>
+  </si>
+  <si>
+    <t>L9493</t>
+  </si>
+  <si>
+    <t>J4403</t>
+  </si>
+  <si>
+    <t>h3233</t>
+  </si>
+  <si>
+    <t>P5592</t>
+  </si>
+  <si>
+    <t>f6700</t>
+  </si>
+  <si>
+    <t>A3107</t>
+  </si>
+  <si>
+    <t>K4561</t>
+  </si>
+  <si>
+    <t>M8875</t>
+  </si>
+  <si>
+    <t>T6859</t>
+  </si>
+  <si>
+    <t>H8058</t>
+  </si>
+  <si>
+    <t>O4499</t>
+  </si>
+  <si>
+    <t>F2829</t>
+  </si>
+  <si>
+    <t>P5904</t>
+  </si>
+  <si>
+    <t>H2288</t>
+  </si>
+  <si>
+    <t>K7056</t>
+  </si>
+  <si>
+    <t>P9512</t>
+  </si>
+  <si>
+    <t>B2286</t>
+  </si>
+  <si>
+    <t>s6696</t>
   </si>
 </sst>
 </file>
@@ -457,99 +535,102 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE9010F3-437C-4CAA-8DE6-817670C40E52}">
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="N38" sqref="N38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>7</v>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
       </c>
       <c r="B2">
         <v>7</v>
       </c>
       <c r="C2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D2">
         <v>5</v>
       </c>
       <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2">
         <v>9</v>
       </c>
-      <c r="F2">
-        <v>8</v>
-      </c>
       <c r="G2">
         <v>8</v>
       </c>
       <c r="H2">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="I2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J2">
+        <v>4</v>
+      </c>
+      <c r="K2">
         <v>10</v>
       </c>
-      <c r="K2">
-        <v>2</v>
-      </c>
       <c r="L2">
         <v>2</v>
       </c>
-      <c r="M2" s="1">
+      <c r="M2">
+        <v>2</v>
+      </c>
+      <c r="N2" s="1">
         <v>0.7142857142857143</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>6</v>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
       </c>
       <c r="B3">
         <v>6</v>
@@ -561,51 +642,54 @@
         <v>6</v>
       </c>
       <c r="E3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F3">
         <v>7</v>
       </c>
       <c r="G3">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H3">
         <v>5</v>
       </c>
       <c r="I3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J3">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="K3">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="L3">
-        <v>1</v>
-      </c>
-      <c r="M3" s="2">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3" s="2">
         <v>0.2857142857142857</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
         <v>10</v>
       </c>
-      <c r="D4">
-        <v>7</v>
-      </c>
       <c r="E4">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G4">
         <v>5</v>
@@ -614,24 +698,27 @@
         <v>5</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
         <v>20</v>
       </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
       <c r="L4">
         <v>0</v>
       </c>
-      <c r="M4" s="2">
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4" s="2">
         <v>0.42857142857142855</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>6</v>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
       </c>
       <c r="B5">
         <v>6</v>
@@ -640,139 +727,148 @@
         <v>6</v>
       </c>
       <c r="D5">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E5">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F5">
         <v>8</v>
       </c>
       <c r="G5">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H5">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I5">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J5">
         <v>5</v>
       </c>
       <c r="K5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L5">
         <v>0</v>
       </c>
-      <c r="M5" s="2">
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5" s="2">
         <v>0.5714285714285714</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
       <c r="C6">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D6">
         <v>7</v>
       </c>
       <c r="E6">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F6">
         <v>5</v>
       </c>
       <c r="G6">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H6">
         <v>7</v>
       </c>
       <c r="I6">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="J6">
+        <v>2</v>
+      </c>
+      <c r="K6">
         <v>10</v>
       </c>
-      <c r="K6">
-        <v>2</v>
-      </c>
       <c r="L6">
-        <v>0</v>
-      </c>
-      <c r="M6" s="2">
+        <v>2</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6" s="2">
         <v>0.5714285714285714</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>3</v>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>18</v>
       </c>
       <c r="B7">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C7">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D7">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F7">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G7">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H7">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J7">
+        <v>4</v>
+      </c>
+      <c r="K7">
         <v>15</v>
       </c>
-      <c r="K7">
-        <v>3</v>
-      </c>
       <c r="L7">
-        <v>1</v>
-      </c>
-      <c r="M7" s="2">
+        <v>3</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7" s="2">
         <v>0.5714285714285714</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>4</v>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>19</v>
       </c>
       <c r="B8">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E8">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F8">
         <v>6</v>
       </c>
       <c r="G8">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H8">
         <v>4</v>
@@ -781,112 +877,121 @@
         <v>4</v>
       </c>
       <c r="J8">
+        <v>4</v>
+      </c>
+      <c r="K8">
         <v>10</v>
       </c>
-      <c r="K8">
-        <v>2</v>
-      </c>
       <c r="L8">
-        <v>0</v>
-      </c>
-      <c r="M8" s="2">
+        <v>2</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8" s="2">
         <v>0.5714285714285714</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>7</v>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>20</v>
       </c>
       <c r="B9">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C9">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D9">
         <v>5</v>
       </c>
       <c r="E9">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F9">
         <v>8</v>
       </c>
       <c r="G9">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="H9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J9">
+        <v>3</v>
+      </c>
+      <c r="K9">
         <v>10</v>
       </c>
-      <c r="K9">
-        <v>6</v>
-      </c>
       <c r="L9">
-        <v>1</v>
-      </c>
-      <c r="M9" s="2">
+        <v>6</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="N9" s="2">
         <v>0.7142857142857143</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>6</v>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>21</v>
       </c>
       <c r="B10">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10">
         <v>7</v>
       </c>
       <c r="D10">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E10">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F10">
+        <v>8</v>
+      </c>
+      <c r="G10">
         <v>9</v>
       </c>
-      <c r="G10">
-        <v>4</v>
-      </c>
       <c r="H10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
         <v>15</v>
       </c>
-      <c r="K10">
-        <v>4</v>
-      </c>
       <c r="L10">
-        <v>5</v>
-      </c>
-      <c r="M10" s="2">
+        <v>4</v>
+      </c>
+      <c r="M10">
+        <v>5</v>
+      </c>
+      <c r="N10" s="2">
         <v>0.8571428571428571</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>4</v>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>22</v>
       </c>
       <c r="B11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C11">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D11">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E11">
         <v>7</v>
@@ -898,83 +1003,89 @@
         <v>7</v>
       </c>
       <c r="H11">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I11">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J11">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K11">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L11">
-        <v>2</v>
-      </c>
-      <c r="M11" s="2">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>2</v>
+      </c>
+      <c r="N11" s="2">
         <v>0.42857142857142855</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>2</v>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>23</v>
       </c>
       <c r="B12">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C12">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D12">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E12">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F12">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G12">
         <v>7</v>
       </c>
       <c r="H12">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="I12">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
         <v>30</v>
       </c>
-      <c r="K12">
-        <v>5</v>
-      </c>
       <c r="L12">
-        <v>1</v>
-      </c>
-      <c r="M12" s="2">
+        <v>5</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12" s="2">
         <v>0.42857142857142855</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>3</v>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>24</v>
       </c>
       <c r="B13">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C13">
+        <v>5</v>
+      </c>
+      <c r="D13">
         <v>9</v>
       </c>
-      <c r="D13">
-        <v>7</v>
-      </c>
       <c r="E13">
         <v>7</v>
       </c>
       <c r="F13">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G13">
         <v>6</v>
@@ -983,24 +1094,27 @@
         <v>6</v>
       </c>
       <c r="I13">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13">
         <v>20</v>
       </c>
-      <c r="K13">
-        <v>3</v>
-      </c>
       <c r="L13">
-        <v>1</v>
-      </c>
-      <c r="M13" s="2">
+        <v>3</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13" s="2">
         <v>0.5714285714285714</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>5</v>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>25</v>
       </c>
       <c r="B14">
         <v>5</v>
@@ -1012,7 +1126,7 @@
         <v>5</v>
       </c>
       <c r="E14">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F14">
         <v>7</v>
@@ -1024,36 +1138,39 @@
         <v>7</v>
       </c>
       <c r="I14">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
         <v>20</v>
       </c>
-      <c r="K14">
-        <v>2</v>
-      </c>
       <c r="L14">
-        <v>1</v>
-      </c>
-      <c r="M14" s="2">
+        <v>2</v>
+      </c>
+      <c r="M14">
+        <v>1</v>
+      </c>
+      <c r="N14" s="2">
         <v>0.42857142857142855</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>6</v>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>26</v>
       </c>
       <c r="B15">
         <v>6</v>
       </c>
       <c r="C15">
+        <v>6</v>
+      </c>
+      <c r="D15">
         <v>9</v>
       </c>
-      <c r="D15">
-        <v>8</v>
-      </c>
       <c r="E15">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F15">
         <v>7</v>
@@ -1065,71 +1182,77 @@
         <v>7</v>
       </c>
       <c r="I15">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="J15">
+        <v>3</v>
+      </c>
+      <c r="K15">
         <v>10</v>
       </c>
-      <c r="K15">
-        <v>2</v>
-      </c>
       <c r="L15">
-        <v>0</v>
-      </c>
-      <c r="M15" s="2">
+        <v>2</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15" s="2">
         <v>0.42857142857142855</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>3</v>
+        <v>8415</v>
       </c>
       <c r="B16">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C16">
+        <v>6</v>
+      </c>
+      <c r="D16">
         <v>9</v>
       </c>
-      <c r="D16">
-        <v>5</v>
-      </c>
       <c r="E16">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F16">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G16">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H16">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="K16">
         <v>35</v>
       </c>
-      <c r="K16">
-        <v>2</v>
-      </c>
       <c r="L16">
-        <v>0</v>
-      </c>
-      <c r="M16" s="2">
+        <v>2</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16" s="2">
         <v>0.7142857142857143</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>6</v>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>27</v>
       </c>
       <c r="B17">
         <v>6</v>
       </c>
       <c r="C17">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D17">
         <v>8</v>
@@ -1141,48 +1264,51 @@
         <v>8</v>
       </c>
       <c r="G17">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H17">
         <v>7</v>
       </c>
       <c r="I17">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J17">
+        <v>5</v>
+      </c>
+      <c r="K17">
         <v>15</v>
       </c>
-      <c r="K17">
-        <v>2</v>
-      </c>
       <c r="L17">
-        <v>0</v>
-      </c>
-      <c r="M17" s="2">
+        <v>2</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17" s="2">
         <v>0.8571428571428571</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18">
         <v>9</v>
       </c>
-      <c r="B18">
-        <v>8</v>
-      </c>
       <c r="C18">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D18">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E18">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F18">
         <v>9</v>
       </c>
       <c r="G18">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="H18">
         <v>2</v>
@@ -1191,57 +1317,350 @@
         <v>2</v>
       </c>
       <c r="J18">
+        <v>2</v>
+      </c>
+      <c r="K18">
         <v>10</v>
       </c>
-      <c r="K18">
-        <v>0</v>
-      </c>
       <c r="L18">
-        <v>5</v>
-      </c>
-      <c r="M18" s="2">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>5</v>
+      </c>
+      <c r="N18" s="2">
         <v>0.5714285714285714</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>4</v>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>29</v>
       </c>
       <c r="B19">
         <v>4</v>
       </c>
       <c r="C19">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D19">
         <v>5</v>
       </c>
       <c r="E19">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F19">
         <v>8</v>
       </c>
       <c r="G19">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H19">
         <v>5</v>
       </c>
       <c r="I19">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="J19">
+        <v>8</v>
+      </c>
+      <c r="K19">
         <v>10</v>
       </c>
-      <c r="K19">
-        <v>1</v>
-      </c>
       <c r="L19">
-        <v>0</v>
-      </c>
-      <c r="M19" s="2">
+        <v>1</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19" s="2">
         <v>0.7142857142857143</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>4</v>
+      </c>
+      <c r="D20">
+        <v>8</v>
+      </c>
+      <c r="E20">
+        <v>7</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+      <c r="K20">
+        <v>5</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="J21">
+        <v>1</v>
+      </c>
+      <c r="K21">
+        <v>5</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22">
+        <v>4</v>
+      </c>
+      <c r="D22">
+        <v>10</v>
+      </c>
+      <c r="E22">
+        <v>7</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+      <c r="K22">
+        <v>13</v>
+      </c>
+      <c r="L22">
+        <v>1</v>
+      </c>
+      <c r="M22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <v>4</v>
+      </c>
+      <c r="D23">
+        <v>10</v>
+      </c>
+      <c r="E23">
+        <v>9</v>
+      </c>
+      <c r="J23">
+        <v>2</v>
+      </c>
+      <c r="K23">
+        <v>20</v>
+      </c>
+      <c r="L23">
+        <v>2</v>
+      </c>
+      <c r="M23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24">
+        <v>3</v>
+      </c>
+      <c r="E24">
+        <v>3</v>
+      </c>
+      <c r="J24">
+        <v>5</v>
+      </c>
+      <c r="K24">
+        <v>10</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25">
+        <v>4</v>
+      </c>
+      <c r="C25">
+        <v>5</v>
+      </c>
+      <c r="D25">
+        <v>10</v>
+      </c>
+      <c r="E25">
+        <v>6</v>
+      </c>
+      <c r="J25">
+        <v>3</v>
+      </c>
+      <c r="K25">
+        <v>20</v>
+      </c>
+      <c r="L25">
+        <v>6</v>
+      </c>
+      <c r="M25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26">
+        <v>3</v>
+      </c>
+      <c r="C26">
+        <v>6</v>
+      </c>
+      <c r="D26">
+        <v>10</v>
+      </c>
+      <c r="E26">
+        <v>8</v>
+      </c>
+      <c r="J26">
+        <v>2</v>
+      </c>
+      <c r="K26">
+        <v>7</v>
+      </c>
+      <c r="L26">
+        <v>2</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27">
+        <v>5</v>
+      </c>
+      <c r="C27">
+        <v>5</v>
+      </c>
+      <c r="D27">
+        <v>6</v>
+      </c>
+      <c r="E27">
+        <v>8</v>
+      </c>
+      <c r="J27">
+        <v>2</v>
+      </c>
+      <c r="K27">
+        <v>5</v>
+      </c>
+      <c r="M27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28">
+        <v>4</v>
+      </c>
+      <c r="C28">
+        <v>5</v>
+      </c>
+      <c r="D28">
+        <v>10</v>
+      </c>
+      <c r="E28">
+        <v>7</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
+      <c r="K28">
+        <v>6</v>
+      </c>
+      <c r="L28">
+        <v>2</v>
+      </c>
+      <c r="M28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>9</v>
+      </c>
+      <c r="C29">
+        <v>8</v>
+      </c>
+      <c r="D29">
+        <v>3</v>
+      </c>
+      <c r="E29">
+        <v>4</v>
+      </c>
+      <c r="J29">
+        <v>2</v>
+      </c>
+      <c r="K29">
+        <v>10</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="M29">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>